<commit_message>
Made all the Filler Words in each voice
</commit_message>
<xml_diff>
--- a/Stims/Filler List Pairings.xlsx
+++ b/Stims/Filler List Pairings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\Social.Influence_Speech.Perception\SI.SP\Stims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6E0AD14-C0E2-40FB-9EB4-691BC146DD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38664B7-AB3F-42D0-80DC-C5BCAF71CF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{789F790E-3DA6-4EEC-A37D-80BD26F72BF3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>40 Male Words</t>
   </si>
@@ -119,13 +119,40 @@
   </si>
   <si>
     <t>Unique Word Pairs</t>
+  </si>
+  <si>
+    <t>(Materials A)</t>
+  </si>
+  <si>
+    <t>(Materials B)</t>
+  </si>
+  <si>
+    <t>Total unique audio files: 160</t>
+  </si>
+  <si>
+    <t>Unique Filler Words: 80</t>
+  </si>
+  <si>
+    <t>Unique Filler Nonwords: 80</t>
+  </si>
+  <si>
+    <t>40 --&gt; Materials A</t>
+  </si>
+  <si>
+    <t>40 --&gt; Materials B</t>
+  </si>
+  <si>
+    <t>Total mono files: 320</t>
+  </si>
+  <si>
+    <t>Total stereo files: 320 (?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +168,13 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Sylfaen"/>
@@ -225,15 +259,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -310,25 +335,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -340,19 +376,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -361,47 +394,59 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,10 +768,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F82010E-5914-4E94-B019-90E817F5CE15}">
-  <dimension ref="A2:U29"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -754,37 +802,37 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="21" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="O2" s="21" t="s">
+      <c r="M2" s="27"/>
+      <c r="O2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="28" t="s">
+      <c r="P2" s="27"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="28"/>
+      <c r="S2" s="27"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="2">
-        <v>20</v>
-      </c>
-      <c r="C3" s="3">
-        <v>20</v>
-      </c>
-      <c r="E3" s="4">
-        <v>20</v>
-      </c>
-      <c r="F3" s="5">
-        <v>20</v>
+      <c r="B3" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>25</v>
@@ -826,11 +874,18 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="2">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4">
+        <v>20</v>
+      </c>
+      <c r="F5" s="5">
+        <v>20</v>
+      </c>
       <c r="I5" s="2" t="s">
         <v>4</v>
       </c>
@@ -857,30 +912,30 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B7" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="26"/>
       <c r="I7" s="3" t="s">
         <v>6</v>
@@ -908,28 +963,18 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="2">
-        <v>20</v>
-      </c>
-      <c r="C9" s="5">
-        <v>20</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="4">
-        <v>20</v>
-      </c>
-      <c r="F9" s="3">
-        <v>20</v>
-      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
       <c r="I9" s="4" t="s">
         <v>7</v>
       </c>
@@ -956,51 +1001,69 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="A10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="5">
+        <v>20</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5">
-        <v>20</v>
-      </c>
-      <c r="D11" s="18" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="I11" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="27"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="O11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" s="27"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20</v>
+      </c>
+      <c r="C12" s="5">
+        <v>20</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4">
-        <v>20</v>
-      </c>
-      <c r="F11" s="3">
-        <v>20</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="21"/>
-      <c r="O11" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="21"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="S11" s="28"/>
-    </row>
-    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E12" s="4">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3">
+        <v>20</v>
+      </c>
       <c r="I12" s="11" t="s">
         <v>24</v>
       </c>
@@ -1026,26 +1089,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-    </row>
-    <row r="14" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="22"/>
+    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="30"/>
+      <c r="B13" s="32"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
         <v>4</v>
@@ -1072,32 +1125,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
-      <c r="B15" s="2">
-        <v>20</v>
-      </c>
-      <c r="C15" s="5">
-        <v>20</v>
-      </c>
-      <c r="E15" s="4">
-        <v>20</v>
-      </c>
-      <c r="F15" s="3">
-        <v>20</v>
-      </c>
+    <row r="15" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="22"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="1:19" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
-      <c r="B16" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="E16" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="23"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B16" s="2">
+        <v>20</v>
+      </c>
+      <c r="C16" s="5">
+        <v>20</v>
+      </c>
+      <c r="E16" s="4">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3">
+        <v>20</v>
+      </c>
       <c r="H16" s="8"/>
       <c r="I16" s="3" t="s">
         <v>6</v>
@@ -1124,31 +1177,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B17" s="2">
-        <v>20</v>
-      </c>
-      <c r="C17" s="5">
-        <v>20</v>
-      </c>
-      <c r="E17" s="4">
-        <v>20</v>
-      </c>
-      <c r="F17" s="3">
-        <v>20</v>
-      </c>
+    <row r="17" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="17"/>
+      <c r="B17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="E17" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="20"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A18" s="19"/>
-      <c r="B18" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="23"/>
-      <c r="E18" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="23"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="2">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5">
+        <v>20</v>
+      </c>
+      <c r="E18" s="4">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3">
+        <v>20</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="4" t="s">
         <v>7</v>
@@ -1176,133 +1230,212 @@
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5">
-        <v>20</v>
-      </c>
-      <c r="C19" s="2">
-        <v>20</v>
-      </c>
-      <c r="E19" s="3">
-        <v>20</v>
-      </c>
-      <c r="F19" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
-      <c r="B20" s="23" t="s">
+      <c r="B19" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="E19" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="20"/>
+    </row>
+    <row r="20" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="17"/>
+      <c r="B20" s="5">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2">
+        <v>20</v>
+      </c>
+      <c r="E20" s="3">
+        <v>20</v>
+      </c>
+      <c r="F20" s="4">
+        <v>20</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+    </row>
+    <row r="21" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+      <c r="B21" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="E20" s="23" t="s">
+      <c r="C21" s="20"/>
+      <c r="E21" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B21" s="5">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2">
-        <v>20</v>
-      </c>
-      <c r="E21" s="3">
-        <v>20</v>
-      </c>
-      <c r="F21" s="4">
-        <v>20</v>
-      </c>
+      <c r="F21" s="20"/>
+      <c r="I21" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="13"/>
+    </row>
+    <row r="22" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7"/>
+      <c r="B22" s="5">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <v>20</v>
+      </c>
+      <c r="E22" s="3">
+        <v>20</v>
+      </c>
+      <c r="F22" s="4">
+        <v>20</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="29"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B23" s="13"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="C24" s="29" t="s">
+      <c r="B24" s="12"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="I24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C25" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-    </row>
-    <row r="25" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="C28:E29"/>
+  <mergeCells count="29">
     <mergeCell ref="R2:S2"/>
+    <mergeCell ref="I20:S20"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q21:S21"/>
+    <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O11:P11"/>
     <mergeCell ref="R11:S11"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C24:E25"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="O24:S24"/>
+    <mergeCell ref="C29:E30"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C25:E26"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B8:F8"/>
     <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="64" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>